<commit_message>
second test failed gateway error
</commit_message>
<xml_diff>
--- a/top100BokksByMedium.xlsx
+++ b/top100BokksByMedium.xlsx
@@ -391,6 +391,13 @@
           <t>F. Scott Fitzgerald</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.91
+</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -408,6 +415,13 @@
           <t>Joseph Heller</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -425,6 +439,11 @@
           <t>Jack Kerouac</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -442,6 +461,13 @@
           <t xml:space="preserve">Harper Lee </t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.27
+</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -459,6 +485,13 @@
           <t>J. R. R. Tolkien</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.50
+</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -476,6 +509,11 @@
           <t>Nabokov</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -493,6 +531,13 @@
           <t xml:space="preserve">JD Salinger </t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.80
+</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -510,6 +555,13 @@
           <t>Salman Rushdie</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -527,6 +579,13 @@
           <t xml:space="preserve">Lewis Carroll </t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.02
+</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -544,6 +603,13 @@
           <t xml:space="preserve">James Joyce </t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.73
+</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -561,6 +627,13 @@
           <t>William Golding</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.68
+</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -578,6 +651,13 @@
           <t>John Steinbeck</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.96
+</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -595,6 +675,13 @@
           <t>George Orwell</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.18
+</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -612,6 +699,13 @@
           <t>Charlotte Brontë</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.12
+</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -629,6 +723,13 @@
           <t>Herman Melville</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.49
+</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -646,6 +747,13 @@
           <t xml:space="preserve">Virginia Woolf </t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.79
+</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -663,6 +771,13 @@
           <t>EM Forster</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.68
+</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -680,6 +795,13 @@
           <t>Aldous Huxley</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -697,6 +819,13 @@
           <t>Chinua Achebe</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.66
+</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -714,6 +843,13 @@
           <t>Muriel Spark</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.74
+</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -731,6 +867,13 @@
           <t>Gabriel García Márquez</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.07
+</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -748,6 +891,13 @@
           <t>Jane Austen</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.26
+</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -765,6 +915,13 @@
           <t>George Orwell</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.93
+</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -782,6 +939,13 @@
           <t>Fyodor Dostoyevsky</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.00
+</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -799,6 +963,13 @@
           <t>Toni Morrison</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.83
+</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -816,6 +987,13 @@
           <t>Ralph Ellison</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.86
+</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -833,6 +1011,13 @@
           <t>Kurt Vonnegut</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.07
+</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -850,6 +1035,13 @@
           <t>Albert Camus</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -867,6 +1059,13 @@
           <t>Miguel De Cervantes</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.87
+</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -884,6 +1083,13 @@
           <t>Daniel Defoe</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.67
+</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -901,6 +1107,13 @@
           <t>Mary Shelley</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.79
+</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -918,6 +1131,13 @@
           <t xml:space="preserve">Alexandre Dumas </t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.24
+</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -935,6 +1155,13 @@
           <t>Charles Dickens</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -952,6 +1179,13 @@
           <t>Emily Brontë</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.85
+</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -969,6 +1203,13 @@
           <t>Louisa M Alcott</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.07
+</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -986,6 +1227,13 @@
           <t>Jack London</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.86
+</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1003,6 +1251,13 @@
           <t>Kenneth Grahame</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.99
+</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1020,6 +1275,13 @@
           <t>Evelyn Waugh</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.85
+</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1037,6 +1299,13 @@
           <t>Raymond Chandler</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.01
+</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1054,6 +1323,13 @@
           <t>Kingsley Amis</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.78
+</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1071,6 +1347,13 @@
           <t>Italo Calvino</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.05
+</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1088,6 +1371,13 @@
           <t>V. S. Naipaul</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.77
+</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1105,6 +1395,13 @@
           <t>Marilynne Robinson</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.82
+</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1122,6 +1419,13 @@
           <t>Ian McEwan</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.90
+</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1139,6 +1443,11 @@
           <t>Philip Pullman</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1156,6 +1465,13 @@
           <t>Douglas Adams</t>
         </is>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.51
+</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1173,6 +1489,13 @@
           <t>Charles Dickens</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.77
+</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1190,6 +1513,13 @@
           <t xml:space="preserve">George Eliot </t>
         </is>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.96
+</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1207,6 +1537,13 @@
           <t>Evelyn Waugh</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.00
+</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1224,6 +1561,13 @@
           <t>Leo Tolstoy</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.05
+</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1241,6 +1585,11 @@
           <t>Philip Roth</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1258,6 +1607,13 @@
           <t>Edith Wharton</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.95
+</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1275,6 +1631,13 @@
           <t>Margaret Atwood</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.10
+</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1292,6 +1655,13 @@
           <t>Ernest Hemingway</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.82
+</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1309,6 +1679,13 @@
           <t xml:space="preserve">Virginia Woolf </t>
         </is>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.78
+</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1326,6 +1703,13 @@
           <t>Don DeLillo</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.87
+</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1343,6 +1727,13 @@
           <t>Carson McCullers</t>
         </is>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.98
+</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1360,6 +1751,13 @@
           <t>William Faulkner</t>
         </is>
       </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.86
+</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1377,6 +1775,13 @@
           <t>Vladimir Nabokov</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.15
+</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1394,6 +1799,13 @@
           <t>Robert Graves</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.27
+</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1411,6 +1823,13 @@
           <t>James Baldwin</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.02
+</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1428,6 +1847,13 @@
           <t>Anthony Powell</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.44
+</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1445,6 +1871,11 @@
           <t xml:space="preserve">Henry Miller </t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1462,6 +1893,13 @@
           <t>Jean Rhys</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.58
+</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1479,6 +1917,13 @@
           <t xml:space="preserve">Iris Murdoch </t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.77
+</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1496,6 +1941,13 @@
           <t>Jonathan Swift</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.57
+</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1513,6 +1965,13 @@
           <t>Henry Fielding</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.74
+</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1530,6 +1989,13 @@
           <t>Samuel Richardson</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.36
+</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1547,6 +2013,13 @@
           <t xml:space="preserve">Laurence Sterne </t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.74
+</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1564,6 +2037,13 @@
           <t xml:space="preserve">Nathaniel Hawthorne </t>
         </is>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.40
+</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1581,6 +2061,13 @@
           <t xml:space="preserve">Gustave Flaubert </t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.67
+</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1598,6 +2085,13 @@
           <t>Henry James</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.77
+</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1615,6 +2109,13 @@
           <t>Robert Louis Stevenson</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.81
+</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1632,6 +2133,13 @@
           <t>Joseph Conrad</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.82
+</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1649,6 +2157,13 @@
           <t>Marcel Proust</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.34
+</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1666,6 +2181,13 @@
           <t>D. H. Lawrence</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.69
+</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1683,6 +2205,11 @@
           <t>Ford Madox Ford</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>3.76</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1700,6 +2227,13 @@
           <t>Franz Kafka</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.97
+</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1717,6 +2251,13 @@
           <t>William Faulkner</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.71
+</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1734,6 +2275,13 @@
           <t>E. B. White</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  4.17
+</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1751,6 +2299,13 @@
           <t xml:space="preserve">Gunter Grass </t>
         </is>
       </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  3.96
+</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1766,6 +2321,11 @@
       <c r="C83" t="inlineStr">
         <is>
           <t>Saul Bellow</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Error</t>
         </is>
       </c>
     </row>

</xml_diff>